<commit_message>
add twitch data test
</commit_message>
<xml_diff>
--- a/test_results/stocks.xlsx
+++ b/test_results/stocks.xlsx
@@ -11,15 +11,14 @@
     <sheet name="module-bodywsodmost-popular-st" sheetId="2" r:id="rId2"/>
     <sheet name="module-bodywsodgainers" sheetId="3" r:id="rId3"/>
     <sheet name="module-bodywsodlosers" sheetId="4" r:id="rId4"/>
-    <sheet name="module-bodywsodcommodities" sheetId="5" r:id="rId5"/>
-    <sheet name="module-bodywsodcurrencies" sheetId="6" r:id="rId6"/>
+    <sheet name="module-bodywsodcurrencies" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="62">
   <si>
     <t>ticker-name</t>
   </si>
@@ -42,31 +41,31 @@
     <t>S&amp;P</t>
   </si>
   <si>
-    <t>0.63%</t>
-  </si>
-  <si>
-    <t>0.50%</t>
-  </si>
-  <si>
-    <t>0.94%</t>
-  </si>
-  <si>
-    <t>35,629.33</t>
-  </si>
-  <si>
-    <t>14,417.55</t>
-  </si>
-  <si>
-    <t>4,589.38</t>
-  </si>
-  <si>
-    <t>224.09</t>
-  </si>
-  <si>
-    <t>71.54</t>
-  </si>
-  <si>
-    <t>42.84</t>
+    <t>-0.67%</t>
+  </si>
+  <si>
+    <t>-1.77%</t>
+  </si>
+  <si>
+    <t>-1.15%</t>
+  </si>
+  <si>
+    <t>35,391.50</t>
+  </si>
+  <si>
+    <t>14,162.95</t>
+  </si>
+  <si>
+    <t>4,536.51</t>
+  </si>
+  <si>
+    <t>-237.83</t>
+  </si>
+  <si>
+    <t>-254.60</t>
+  </si>
+  <si>
+    <t>-52.87</t>
   </si>
   <si>
     <t>column</t>
@@ -81,37 +80,37 @@
     <t>Twitter Inc</t>
   </si>
   <si>
-    <t>Macy's Inc</t>
-  </si>
-  <si>
-    <t>Alibaba Group Holding Ltd</t>
-  </si>
-  <si>
-    <t>Southwest Airlines Co</t>
-  </si>
-  <si>
-    <t>36.52</t>
-  </si>
-  <si>
-    <t>25.27</t>
-  </si>
-  <si>
-    <t>122.78</t>
-  </si>
-  <si>
-    <t>44.29</t>
-  </si>
-  <si>
-    <t>-4.20%</t>
-  </si>
-  <si>
-    <t>-3.55%</t>
-  </si>
-  <si>
-    <t>-3.49%</t>
-  </si>
-  <si>
-    <t>-1.97%</t>
+    <t>Chipotle Mexican Grill Inc</t>
+  </si>
+  <si>
+    <t>Visa Inc</t>
+  </si>
+  <si>
+    <t>Walt Disney Co</t>
+  </si>
+  <si>
+    <t>34.20</t>
+  </si>
+  <si>
+    <t>1,453.23</t>
+  </si>
+  <si>
+    <t>232.39</t>
+  </si>
+  <si>
+    <t>140.80</t>
+  </si>
+  <si>
+    <t>-6.33%</t>
+  </si>
+  <si>
+    <t>-2.11%</t>
+  </si>
+  <si>
+    <t>-1.29%</t>
+  </si>
+  <si>
+    <t>-1.28%</t>
   </si>
   <si>
     <t>hidden</t>
@@ -150,76 +149,31 @@
     <t>0.00</t>
   </si>
   <si>
-    <t>Boston Scientific Corp</t>
-  </si>
-  <si>
-    <t>IDEX Corp</t>
-  </si>
-  <si>
-    <t>Paycom Software Inc</t>
-  </si>
-  <si>
-    <t>Gap Inc</t>
-  </si>
-  <si>
-    <t>-4.74%</t>
-  </si>
-  <si>
-    <t>-4.50%</t>
-  </si>
-  <si>
-    <t>-4.22%</t>
-  </si>
-  <si>
-    <t>-3.69%</t>
-  </si>
-  <si>
-    <t>-3.28%</t>
-  </si>
-  <si>
-    <t>Oil</t>
-  </si>
-  <si>
-    <t>Gas</t>
-  </si>
-  <si>
-    <t>Gold</t>
-  </si>
-  <si>
-    <t>Silver</t>
-  </si>
-  <si>
-    <t>Corn</t>
-  </si>
-  <si>
-    <t>$87.71</t>
-  </si>
-  <si>
-    <t>$5.28</t>
-  </si>
-  <si>
-    <t>$1,806.10</t>
-  </si>
-  <si>
-    <t>$22.54</t>
-  </si>
-  <si>
-    <t>$619.25</t>
-  </si>
-  <si>
-    <t>-0.62%</t>
-  </si>
-  <si>
-    <t>-3.96%</t>
-  </si>
-  <si>
-    <t>-0.23%</t>
-  </si>
-  <si>
-    <t>-0.76%</t>
-  </si>
-  <si>
-    <t>-0.52%</t>
+    <t>Xylem Inc</t>
+  </si>
+  <si>
+    <t>Fortive Corp</t>
+  </si>
+  <si>
+    <t>Epam Systems Inc</t>
+  </si>
+  <si>
+    <t>Salesforce.Com Inc</t>
+  </si>
+  <si>
+    <t>-9.82%</t>
+  </si>
+  <si>
+    <t>-6.00%</t>
+  </si>
+  <si>
+    <t>-5.81%</t>
+  </si>
+  <si>
+    <t>-4.77%</t>
+  </si>
+  <si>
+    <t>-4.75%</t>
   </si>
   <si>
     <t>British Pound</t>
@@ -940,7 +894,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
         <v>48</v>
@@ -954,7 +908,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
         <v>49</v>
@@ -1011,114 +965,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -1139,10 +985,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1150,10 +996,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1161,10 +1007,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1172,10 +1018,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1183,10 +1029,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>